<commit_message>
Added variable to separate pretrained and others
</commit_message>
<xml_diff>
--- a/data_exploration/acl/tables/pretrain_size.xlsx
+++ b/data_exploration/acl/tables/pretrain_size.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Language</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>CCGiB</t>
+  </si>
+  <si>
+    <t>Pretrained</t>
   </si>
 </sst>
 </file>
@@ -467,15 +470,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -488,8 +491,11 @@
       <c r="D1" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -502,8 +508,11 @@
       <c r="D2">
         <v>66.599999999999994</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -516,8 +525,11 @@
       <c r="D3">
         <v>53.3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -530,8 +542,11 @@
       <c r="D4">
         <v>23.2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -544,8 +559,11 @@
       <c r="D5">
         <v>49</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -558,8 +576,11 @@
       <c r="D6">
         <v>46.9</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -572,8 +593,11 @@
       <c r="D7">
         <v>63.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -586,8 +610,11 @@
       <c r="D8">
         <v>137.30000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -600,8 +627,11 @@
       <c r="D9">
         <v>71.7</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -614,8 +644,11 @@
       <c r="D10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -628,8 +661,11 @@
       <c r="D11">
         <v>148.30000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -642,8 +678,11 @@
       <c r="D12">
         <v>54.3</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -656,8 +695,11 @@
       <c r="D13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -670,8 +712,11 @@
       <c r="D14">
         <v>54.2</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -684,8 +729,11 @@
       <c r="D15">
         <v>69.3</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -698,8 +746,11 @@
       <c r="D16">
         <v>20.9</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -712,8 +763,11 @@
       <c r="D17">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -726,8 +780,11 @@
       <c r="D18">
         <v>31.6</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -740,8 +797,11 @@
       <c r="D19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -752,6 +812,9 @@
         <v>0</v>
       </c>
       <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
         <v>0</v>
       </c>
     </row>

</xml_diff>